<commit_message>
Update WaaS InPlace Upgrade Pace v 1.2.xlsx
</commit_message>
<xml_diff>
--- a/WaaSProgressSpreadsheet/WaaS InPlace Upgrade Pace v 1.2.xlsx
+++ b/WaaSProgressSpreadsheet/WaaS InPlace Upgrade Pace v 1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\GitHub\BlogFiles\WaaSProgressSpreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EB820F-1ADB-4252-B12D-FEDD35844A5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D601C2-03C6-46FD-AE4B-13E4EDE5C637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -3730,7 +3730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3943,9 +3943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:EK57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13391,8 +13391,8 @@
     </row>
     <row r="23" spans="1:141" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="str">
-        <f>CONCATENATE("Weekly Change [Post-",Variables!B30,"]")</f>
-        <v>Weekly Change [Post-1809]</v>
+        <f>CONCATENATE("Weekly Change [Pre-",Variables!B30,"]")</f>
+        <v>Weekly Change [Pre-1809]</v>
       </c>
       <c r="C23" s="15">
         <f>C20-B20</f>
@@ -14504,8 +14504,8 @@
     </row>
     <row r="26" spans="1:141" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="str">
-        <f>CONCATENATE("Running Change [Post-",Variables!B30,"]")</f>
-        <v>Running Change [Post-1809]</v>
+        <f>CONCATENATE("Running Change [Pre-",Variables!B30,"]")</f>
+        <v>Running Change [Pre-1809]</v>
       </c>
       <c r="C26" s="15">
         <f>C20-$B20</f>
@@ -15617,8 +15617,8 @@
     </row>
     <row r="29" spans="1:141" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="str">
-        <f>CONCATENATE("Average Weekly Change [Post-",Variables!B30,"]")</f>
-        <v>Average Weekly Change [Post-1809]</v>
+        <f>CONCATENATE("Average Weekly Change [Pre-",Variables!B30,"]")</f>
+        <v>Average Weekly Change [Pre-1809]</v>
       </c>
       <c r="C29" s="15">
         <f>C$26/C$42</f>

</xml_diff>